<commit_message>
▶ [24.10.28 15:16] 00. Git 분석 파일 수정(by tamario)
</commit_message>
<xml_diff>
--- a/77_실행_파일_만들기/dist/02. 자산 검증(24.10)_RSLT.xlsx
+++ b/77_실행_파일_만들기/dist/02. 자산 검증(24.10)_RSLT.xlsx
@@ -6698,7 +6698,7 @@
       <c r="D3" s="706" t="n"/>
       <c r="E3" s="707" t="inlineStr">
         <is>
-          <t>2024.10.27</t>
+          <t>2024.10.28</t>
         </is>
       </c>
       <c r="G3" s="708" t="inlineStr">
@@ -11792,7 +11792,7 @@
       <c r="H3" s="709" t="n"/>
       <c r="I3" s="707" t="inlineStr">
         <is>
-          <t>2024.10.27</t>
+          <t>2024.10.28</t>
         </is>
       </c>
     </row>

</xml_diff>